<commit_message>
LAst fix and another run
</commit_message>
<xml_diff>
--- a/media/output/result/sepsis_cases_1_complex_evaluation_weighted_edit_distance.xlsx
+++ b/media/output/result/sepsis_cases_1_complex_evaluation_weighted_edit_distance.xlsx
@@ -592,25 +592,25 @@
         <v>151</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E6" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>135</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.8940397350993378</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>0.9440559440559442</v>
       </c>
     </row>
     <row r="7">
@@ -621,25 +621,25 @@
         <v>151</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E7" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>135</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>0.8940397350993378</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>0.9440559440559442</v>
       </c>
     </row>
     <row r="8">
@@ -650,25 +650,25 @@
         <v>151</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E8" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>135</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>0.8940397350993378</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>0.9440559440559442</v>
       </c>
     </row>
     <row r="9">
@@ -679,25 +679,25 @@
         <v>151</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E9" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>135</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>0.8940397350993378</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>0.9440559440559442</v>
       </c>
     </row>
     <row r="10">
@@ -708,25 +708,25 @@
         <v>148</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E10" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>0.8918918918918919</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>0.9428571428571428</v>
       </c>
     </row>
     <row r="11">
@@ -737,25 +737,25 @@
         <v>146</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E11" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>0.8904109589041096</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>0.9420289855072463</v>
       </c>
     </row>
     <row r="12">
@@ -766,25 +766,25 @@
         <v>135</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>121</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E12" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>121</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>0.8962962962962963</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>0.9453124999999999</v>
       </c>
     </row>
     <row r="13">

</xml_diff>